<commit_message>
Ahora los descuentos se calculan de forma automática
</commit_message>
<xml_diff>
--- a/productos_ejemplo.xlsx
+++ b/productos_ejemplo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sistema\Documentos\GitHub\Xpatl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D6C7FA-B3C7-4E56-8BC2-FC59B7C8A31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773DE1FB-F5A8-4843-A42B-F3F3832984A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11565" yWindow="4230" windowWidth="12330" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7680" yWindow="3510" windowWidth="16200" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
@@ -1573,7 +1573,7 @@
     <t>Precio_lista</t>
   </si>
   <si>
-    <t>Precio_descuento</t>
+    <t>Descuento</t>
   </si>
 </sst>
 </file>
@@ -2418,7 +2418,7 @@
   <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2454,7 +2454,7 @@
         <v>50</v>
       </c>
       <c r="E2">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
         <v>50</v>
       </c>
       <c r="E3">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2488,7 +2488,7 @@
         <v>50</v>
       </c>
       <c r="E4">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2522,7 +2522,7 @@
         <v>50</v>
       </c>
       <c r="E6">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2539,7 +2539,7 @@
         <v>50</v>
       </c>
       <c r="E7">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2556,7 +2556,7 @@
         <v>50</v>
       </c>
       <c r="E8">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2573,7 +2573,7 @@
         <v>50</v>
       </c>
       <c r="E9">
-        <v>25</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2590,7 +2590,7 @@
         <v>50</v>
       </c>
       <c r="E10">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2607,7 +2607,7 @@
         <v>50</v>
       </c>
       <c r="E11">
-        <v>25</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2624,7 +2624,7 @@
         <v>50</v>
       </c>
       <c r="E12">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2641,7 +2641,7 @@
         <v>50</v>
       </c>
       <c r="E13">
-        <v>25</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2658,7 +2658,7 @@
         <v>50</v>
       </c>
       <c r="E14">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2675,7 +2675,7 @@
         <v>50</v>
       </c>
       <c r="E15">
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2692,7 +2692,7 @@
         <v>50</v>
       </c>
       <c r="E16">
-        <v>25</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2709,7 +2709,7 @@
         <v>50</v>
       </c>
       <c r="E17">
-        <v>25</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2726,7 +2726,7 @@
         <v>50</v>
       </c>
       <c r="E18">
-        <v>25</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2743,7 +2743,7 @@
         <v>50</v>
       </c>
       <c r="E19">
-        <v>25</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2760,7 +2760,7 @@
         <v>50</v>
       </c>
       <c r="E20">
-        <v>25</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2777,7 +2777,7 @@
         <v>50</v>
       </c>
       <c r="E21">
-        <v>25</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2794,7 +2794,7 @@
         <v>50</v>
       </c>
       <c r="E22">
-        <v>25</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2811,7 +2811,7 @@
         <v>50</v>
       </c>
       <c r="E23">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2828,7 +2828,7 @@
         <v>50</v>
       </c>
       <c r="E24">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2845,7 +2845,7 @@
         <v>50</v>
       </c>
       <c r="E25">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2862,7 +2862,7 @@
         <v>50</v>
       </c>
       <c r="E26">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2879,7 +2879,7 @@
         <v>50</v>
       </c>
       <c r="E27">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2896,7 +2896,7 @@
         <v>50</v>
       </c>
       <c r="E28">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2913,7 +2913,7 @@
         <v>50</v>
       </c>
       <c r="E29">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2930,7 +2930,7 @@
         <v>50</v>
       </c>
       <c r="E30">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2947,7 +2947,7 @@
         <v>50</v>
       </c>
       <c r="E31">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2964,7 +2964,7 @@
         <v>50</v>
       </c>
       <c r="E32">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2981,7 +2981,7 @@
         <v>50</v>
       </c>
       <c r="E33">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2998,7 +2998,7 @@
         <v>50</v>
       </c>
       <c r="E34">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3015,7 +3015,7 @@
         <v>50</v>
       </c>
       <c r="E35">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3032,7 +3032,7 @@
         <v>50</v>
       </c>
       <c r="E36">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3049,7 +3049,7 @@
         <v>50</v>
       </c>
       <c r="E37">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3066,7 +3066,7 @@
         <v>50</v>
       </c>
       <c r="E38">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3083,7 +3083,7 @@
         <v>50</v>
       </c>
       <c r="E39">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3100,7 +3100,7 @@
         <v>50</v>
       </c>
       <c r="E40">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3117,7 +3117,7 @@
         <v>50</v>
       </c>
       <c r="E41">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3134,7 +3134,7 @@
         <v>50</v>
       </c>
       <c r="E42">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3151,7 +3151,7 @@
         <v>50</v>
       </c>
       <c r="E43">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3168,7 +3168,7 @@
         <v>50</v>
       </c>
       <c r="E44">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3185,7 +3185,7 @@
         <v>50</v>
       </c>
       <c r="E45">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3202,7 +3202,7 @@
         <v>50</v>
       </c>
       <c r="E46">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3219,7 +3219,7 @@
         <v>50</v>
       </c>
       <c r="E47">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3236,7 +3236,7 @@
         <v>50</v>
       </c>
       <c r="E48">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3253,7 +3253,7 @@
         <v>50</v>
       </c>
       <c r="E49">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3270,7 +3270,7 @@
         <v>50</v>
       </c>
       <c r="E50">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3287,7 +3287,7 @@
         <v>50</v>
       </c>
       <c r="E51">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3304,7 +3304,7 @@
         <v>50</v>
       </c>
       <c r="E52">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3321,7 +3321,7 @@
         <v>50</v>
       </c>
       <c r="E53">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3338,7 +3338,7 @@
         <v>50</v>
       </c>
       <c r="E54">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3355,7 +3355,7 @@
         <v>50</v>
       </c>
       <c r="E55">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3372,7 +3372,7 @@
         <v>50</v>
       </c>
       <c r="E56">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3389,7 +3389,7 @@
         <v>50</v>
       </c>
       <c r="E57">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3406,7 +3406,7 @@
         <v>50</v>
       </c>
       <c r="E58">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3423,7 +3423,7 @@
         <v>50</v>
       </c>
       <c r="E59">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3440,7 +3440,7 @@
         <v>50</v>
       </c>
       <c r="E60">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3457,7 +3457,7 @@
         <v>50</v>
       </c>
       <c r="E61">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3474,7 +3474,7 @@
         <v>50</v>
       </c>
       <c r="E62">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3491,7 +3491,7 @@
         <v>50</v>
       </c>
       <c r="E63">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3508,7 +3508,7 @@
         <v>50</v>
       </c>
       <c r="E64">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3525,7 +3525,7 @@
         <v>50</v>
       </c>
       <c r="E65">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3542,7 +3542,7 @@
         <v>50</v>
       </c>
       <c r="E66">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3559,7 +3559,7 @@
         <v>50</v>
       </c>
       <c r="E67">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3576,7 +3576,7 @@
         <v>50</v>
       </c>
       <c r="E68">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3593,7 +3593,7 @@
         <v>50</v>
       </c>
       <c r="E69">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3610,7 +3610,7 @@
         <v>50</v>
       </c>
       <c r="E70">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3627,7 +3627,7 @@
         <v>50</v>
       </c>
       <c r="E71">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3644,7 +3644,7 @@
         <v>50</v>
       </c>
       <c r="E72">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3661,7 +3661,7 @@
         <v>50</v>
       </c>
       <c r="E73">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3678,7 +3678,7 @@
         <v>50</v>
       </c>
       <c r="E74">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3695,7 +3695,7 @@
         <v>50</v>
       </c>
       <c r="E75">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3712,7 +3712,7 @@
         <v>50</v>
       </c>
       <c r="E76">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3729,7 +3729,7 @@
         <v>50</v>
       </c>
       <c r="E77">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3746,7 +3746,7 @@
         <v>50</v>
       </c>
       <c r="E78">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3763,7 +3763,7 @@
         <v>50</v>
       </c>
       <c r="E79">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3780,7 +3780,7 @@
         <v>50</v>
       </c>
       <c r="E80">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3797,7 +3797,7 @@
         <v>50</v>
       </c>
       <c r="E81">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3814,7 +3814,7 @@
         <v>50</v>
       </c>
       <c r="E82">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3831,7 +3831,7 @@
         <v>50</v>
       </c>
       <c r="E83">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3848,7 +3848,7 @@
         <v>50</v>
       </c>
       <c r="E84">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3865,7 +3865,7 @@
         <v>50</v>
       </c>
       <c r="E85">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3882,7 +3882,7 @@
         <v>50</v>
       </c>
       <c r="E86">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3899,7 +3899,7 @@
         <v>50</v>
       </c>
       <c r="E87">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3916,7 +3916,7 @@
         <v>50</v>
       </c>
       <c r="E88">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3933,7 +3933,7 @@
         <v>50</v>
       </c>
       <c r="E89">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -3950,7 +3950,7 @@
         <v>50</v>
       </c>
       <c r="E90">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -3967,7 +3967,7 @@
         <v>50</v>
       </c>
       <c r="E91">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3984,7 +3984,7 @@
         <v>50</v>
       </c>
       <c r="E92">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4001,7 +4001,7 @@
         <v>50</v>
       </c>
       <c r="E93">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -4018,7 +4018,7 @@
         <v>50</v>
       </c>
       <c r="E94">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -4035,7 +4035,7 @@
         <v>50</v>
       </c>
       <c r="E95">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -4052,7 +4052,7 @@
         <v>50</v>
       </c>
       <c r="E96">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -4069,7 +4069,7 @@
         <v>50</v>
       </c>
       <c r="E97">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -4086,7 +4086,7 @@
         <v>50</v>
       </c>
       <c r="E98">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -4103,7 +4103,7 @@
         <v>50</v>
       </c>
       <c r="E99">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -4120,7 +4120,7 @@
         <v>50</v>
       </c>
       <c r="E100">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -4137,7 +4137,7 @@
         <v>50</v>
       </c>
       <c r="E101">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -4154,7 +4154,7 @@
         <v>50</v>
       </c>
       <c r="E102">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -4171,7 +4171,7 @@
         <v>50</v>
       </c>
       <c r="E103">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -4188,7 +4188,7 @@
         <v>50</v>
       </c>
       <c r="E104">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -4205,7 +4205,7 @@
         <v>50</v>
       </c>
       <c r="E105">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -4222,7 +4222,7 @@
         <v>50</v>
       </c>
       <c r="E106">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -4239,7 +4239,7 @@
         <v>50</v>
       </c>
       <c r="E107">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -4256,7 +4256,7 @@
         <v>50</v>
       </c>
       <c r="E108">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -4273,7 +4273,7 @@
         <v>50</v>
       </c>
       <c r="E109">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -4290,7 +4290,7 @@
         <v>50</v>
       </c>
       <c r="E110">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -4307,7 +4307,7 @@
         <v>50</v>
       </c>
       <c r="E111">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -4324,7 +4324,7 @@
         <v>50</v>
       </c>
       <c r="E112">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4341,7 +4341,7 @@
         <v>50</v>
       </c>
       <c r="E113">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4358,7 +4358,7 @@
         <v>50</v>
       </c>
       <c r="E114">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4375,7 +4375,7 @@
         <v>50</v>
       </c>
       <c r="E115">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4392,7 +4392,7 @@
         <v>50</v>
       </c>
       <c r="E116">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4409,7 +4409,7 @@
         <v>50</v>
       </c>
       <c r="E117">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4426,7 +4426,7 @@
         <v>50</v>
       </c>
       <c r="E118">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4443,7 +4443,7 @@
         <v>50</v>
       </c>
       <c r="E119">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4460,7 +4460,7 @@
         <v>50</v>
       </c>
       <c r="E120">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4477,7 +4477,7 @@
         <v>50</v>
       </c>
       <c r="E121">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4494,7 +4494,7 @@
         <v>50</v>
       </c>
       <c r="E122">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4511,7 +4511,7 @@
         <v>50</v>
       </c>
       <c r="E123">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -4528,7 +4528,7 @@
         <v>50</v>
       </c>
       <c r="E124">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4545,7 +4545,7 @@
         <v>50</v>
       </c>
       <c r="E125">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4562,7 +4562,7 @@
         <v>50</v>
       </c>
       <c r="E126">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4579,7 +4579,7 @@
         <v>50</v>
       </c>
       <c r="E127">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4596,7 +4596,7 @@
         <v>50</v>
       </c>
       <c r="E128">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4613,7 +4613,7 @@
         <v>50</v>
       </c>
       <c r="E129">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4630,7 +4630,7 @@
         <v>50</v>
       </c>
       <c r="E130">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4647,7 +4647,7 @@
         <v>50</v>
       </c>
       <c r="E131">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4664,7 +4664,7 @@
         <v>50</v>
       </c>
       <c r="E132">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4681,7 +4681,7 @@
         <v>50</v>
       </c>
       <c r="E133">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4698,7 +4698,7 @@
         <v>50</v>
       </c>
       <c r="E134">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4715,7 +4715,7 @@
         <v>50</v>
       </c>
       <c r="E135">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4732,7 +4732,7 @@
         <v>50</v>
       </c>
       <c r="E136">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4749,7 +4749,7 @@
         <v>50</v>
       </c>
       <c r="E137">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4766,7 +4766,7 @@
         <v>50</v>
       </c>
       <c r="E138">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4783,7 +4783,7 @@
         <v>50</v>
       </c>
       <c r="E139">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4800,7 +4800,7 @@
         <v>50</v>
       </c>
       <c r="E140">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -4817,7 +4817,7 @@
         <v>50</v>
       </c>
       <c r="E141">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -4834,7 +4834,7 @@
         <v>50</v>
       </c>
       <c r="E142">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -4851,7 +4851,7 @@
         <v>50</v>
       </c>
       <c r="E143">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -4868,7 +4868,7 @@
         <v>50</v>
       </c>
       <c r="E144">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -4885,7 +4885,7 @@
         <v>50</v>
       </c>
       <c r="E145">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -4902,7 +4902,7 @@
         <v>50</v>
       </c>
       <c r="E146">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -4919,7 +4919,7 @@
         <v>50</v>
       </c>
       <c r="E147">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -4936,7 +4936,7 @@
         <v>50</v>
       </c>
       <c r="E148">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -4953,7 +4953,7 @@
         <v>50</v>
       </c>
       <c r="E149">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -4970,7 +4970,7 @@
         <v>50</v>
       </c>
       <c r="E150">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -4987,7 +4987,7 @@
         <v>50</v>
       </c>
       <c r="E151">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -5004,7 +5004,7 @@
         <v>50</v>
       </c>
       <c r="E152">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -5021,7 +5021,7 @@
         <v>50</v>
       </c>
       <c r="E153">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -5038,7 +5038,7 @@
         <v>50</v>
       </c>
       <c r="E154">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -5055,7 +5055,7 @@
         <v>50</v>
       </c>
       <c r="E155">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -5072,7 +5072,7 @@
         <v>50</v>
       </c>
       <c r="E156">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -5089,7 +5089,7 @@
         <v>50</v>
       </c>
       <c r="E157">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -5106,7 +5106,7 @@
         <v>50</v>
       </c>
       <c r="E158">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
@@ -5123,7 +5123,7 @@
         <v>50</v>
       </c>
       <c r="E159">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
@@ -5140,7 +5140,7 @@
         <v>50</v>
       </c>
       <c r="E160">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -5157,7 +5157,7 @@
         <v>50</v>
       </c>
       <c r="E161">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -5174,7 +5174,7 @@
         <v>50</v>
       </c>
       <c r="E162">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -5191,7 +5191,7 @@
         <v>50</v>
       </c>
       <c r="E163">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -5208,7 +5208,7 @@
         <v>50</v>
       </c>
       <c r="E164">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -5225,7 +5225,7 @@
         <v>50</v>
       </c>
       <c r="E165">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5242,7 +5242,7 @@
         <v>50</v>
       </c>
       <c r="E166">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5259,7 +5259,7 @@
         <v>50</v>
       </c>
       <c r="E167">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -5276,7 +5276,7 @@
         <v>50</v>
       </c>
       <c r="E168">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -5293,7 +5293,7 @@
         <v>50</v>
       </c>
       <c r="E169">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -5310,7 +5310,7 @@
         <v>50</v>
       </c>
       <c r="E170">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -5327,7 +5327,7 @@
         <v>50</v>
       </c>
       <c r="E171">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -5344,7 +5344,7 @@
         <v>50</v>
       </c>
       <c r="E172">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -5361,7 +5361,7 @@
         <v>50</v>
       </c>
       <c r="E173">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -5378,7 +5378,7 @@
         <v>50</v>
       </c>
       <c r="E174">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -5395,7 +5395,7 @@
         <v>50</v>
       </c>
       <c r="E175">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -5412,7 +5412,7 @@
         <v>50</v>
       </c>
       <c r="E176">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -5429,7 +5429,7 @@
         <v>50</v>
       </c>
       <c r="E177">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -5446,7 +5446,7 @@
         <v>50</v>
       </c>
       <c r="E178">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -5463,7 +5463,7 @@
         <v>50</v>
       </c>
       <c r="E179">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -5480,7 +5480,7 @@
         <v>50</v>
       </c>
       <c r="E180">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -5497,7 +5497,7 @@
         <v>50</v>
       </c>
       <c r="E181">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -5514,7 +5514,7 @@
         <v>50</v>
       </c>
       <c r="E182">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -5531,7 +5531,7 @@
         <v>50</v>
       </c>
       <c r="E183">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -5548,7 +5548,7 @@
         <v>50</v>
       </c>
       <c r="E184">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -5565,7 +5565,7 @@
         <v>50</v>
       </c>
       <c r="E185">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -5582,7 +5582,7 @@
         <v>50</v>
       </c>
       <c r="E186">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -5599,7 +5599,7 @@
         <v>50</v>
       </c>
       <c r="E187">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -5616,7 +5616,7 @@
         <v>50</v>
       </c>
       <c r="E188">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -5633,7 +5633,7 @@
         <v>50</v>
       </c>
       <c r="E189">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -5650,7 +5650,7 @@
         <v>50</v>
       </c>
       <c r="E190">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -5667,7 +5667,7 @@
         <v>50</v>
       </c>
       <c r="E191">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -5684,7 +5684,7 @@
         <v>50</v>
       </c>
       <c r="E192">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -5701,7 +5701,7 @@
         <v>50</v>
       </c>
       <c r="E193">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -5718,7 +5718,7 @@
         <v>50</v>
       </c>
       <c r="E194">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -5735,7 +5735,7 @@
         <v>50</v>
       </c>
       <c r="E195">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -5752,7 +5752,7 @@
         <v>50</v>
       </c>
       <c r="E196">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -5769,7 +5769,7 @@
         <v>50</v>
       </c>
       <c r="E197">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -5786,7 +5786,7 @@
         <v>50</v>
       </c>
       <c r="E198">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -5803,7 +5803,7 @@
         <v>50</v>
       </c>
       <c r="E199">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -5820,7 +5820,7 @@
         <v>50</v>
       </c>
       <c r="E200">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -5837,7 +5837,7 @@
         <v>50</v>
       </c>
       <c r="E201">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -5854,7 +5854,7 @@
         <v>50</v>
       </c>
       <c r="E202">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -5871,7 +5871,7 @@
         <v>50</v>
       </c>
       <c r="E203">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -5888,7 +5888,7 @@
         <v>50</v>
       </c>
       <c r="E204">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -5905,7 +5905,7 @@
         <v>50</v>
       </c>
       <c r="E205">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -5922,7 +5922,7 @@
         <v>50</v>
       </c>
       <c r="E206">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -5939,7 +5939,7 @@
         <v>50</v>
       </c>
       <c r="E207">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -5956,7 +5956,7 @@
         <v>50</v>
       </c>
       <c r="E208">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -5973,7 +5973,7 @@
         <v>50</v>
       </c>
       <c r="E209">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -5990,7 +5990,7 @@
         <v>50</v>
       </c>
       <c r="E210">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -6007,7 +6007,7 @@
         <v>50</v>
       </c>
       <c r="E211">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -6024,7 +6024,7 @@
         <v>50</v>
       </c>
       <c r="E212">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -6041,7 +6041,7 @@
         <v>50</v>
       </c>
       <c r="E213">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -6058,7 +6058,7 @@
         <v>50</v>
       </c>
       <c r="E214">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -6075,7 +6075,7 @@
         <v>50</v>
       </c>
       <c r="E215">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -6092,7 +6092,7 @@
         <v>50</v>
       </c>
       <c r="E216">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -6109,7 +6109,7 @@
         <v>50</v>
       </c>
       <c r="E217">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -6126,7 +6126,7 @@
         <v>50</v>
       </c>
       <c r="E218">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -6143,7 +6143,7 @@
         <v>50</v>
       </c>
       <c r="E219">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -6160,7 +6160,7 @@
         <v>50</v>
       </c>
       <c r="E220">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -6177,7 +6177,7 @@
         <v>50</v>
       </c>
       <c r="E221">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -6194,7 +6194,7 @@
         <v>50</v>
       </c>
       <c r="E222">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -6211,7 +6211,7 @@
         <v>50</v>
       </c>
       <c r="E223">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -6228,7 +6228,7 @@
         <v>50</v>
       </c>
       <c r="E224">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -6245,7 +6245,7 @@
         <v>50</v>
       </c>
       <c r="E225">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -6262,7 +6262,7 @@
         <v>50</v>
       </c>
       <c r="E226">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -6279,7 +6279,7 @@
         <v>50</v>
       </c>
       <c r="E227">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -6296,7 +6296,7 @@
         <v>50</v>
       </c>
       <c r="E228">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -6313,7 +6313,7 @@
         <v>50</v>
       </c>
       <c r="E229">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -6330,7 +6330,7 @@
         <v>50</v>
       </c>
       <c r="E230">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -6347,7 +6347,7 @@
         <v>50</v>
       </c>
       <c r="E231">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -6364,7 +6364,7 @@
         <v>50</v>
       </c>
       <c r="E232">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -6381,7 +6381,7 @@
         <v>50</v>
       </c>
       <c r="E233">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -6398,7 +6398,7 @@
         <v>50</v>
       </c>
       <c r="E234">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -6415,7 +6415,7 @@
         <v>50</v>
       </c>
       <c r="E235">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -6432,7 +6432,7 @@
         <v>50</v>
       </c>
       <c r="E236">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -6449,7 +6449,7 @@
         <v>50</v>
       </c>
       <c r="E237">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -6466,7 +6466,7 @@
         <v>50</v>
       </c>
       <c r="E238">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -6483,7 +6483,7 @@
         <v>50</v>
       </c>
       <c r="E239">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -6500,7 +6500,7 @@
         <v>50</v>
       </c>
       <c r="E240">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -6517,7 +6517,7 @@
         <v>50</v>
       </c>
       <c r="E241">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -6534,7 +6534,7 @@
         <v>50</v>
       </c>
       <c r="E242">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -6551,7 +6551,7 @@
         <v>50</v>
       </c>
       <c r="E243">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -6568,7 +6568,7 @@
         <v>50</v>
       </c>
       <c r="E244">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -6585,7 +6585,7 @@
         <v>50</v>
       </c>
       <c r="E245">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -6602,7 +6602,7 @@
         <v>50</v>
       </c>
       <c r="E246">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -6619,7 +6619,7 @@
         <v>50</v>
       </c>
       <c r="E247">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -6636,7 +6636,7 @@
         <v>50</v>
       </c>
       <c r="E248">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -6653,7 +6653,7 @@
         <v>50</v>
       </c>
       <c r="E249">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -6670,7 +6670,7 @@
         <v>50</v>
       </c>
       <c r="E250">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -6687,7 +6687,7 @@
         <v>50</v>
       </c>
       <c r="E251">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -6704,7 +6704,7 @@
         <v>50</v>
       </c>
       <c r="E252">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -6721,7 +6721,7 @@
         <v>50</v>
       </c>
       <c r="E253">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -6738,7 +6738,7 @@
         <v>50</v>
       </c>
       <c r="E254">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -6755,7 +6755,7 @@
         <v>50</v>
       </c>
       <c r="E255">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -6772,7 +6772,7 @@
         <v>50</v>
       </c>
       <c r="E256">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -6789,7 +6789,7 @@
         <v>50</v>
       </c>
       <c r="E257">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -6806,7 +6806,7 @@
         <v>50</v>
       </c>
       <c r="E258">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -6823,7 +6823,7 @@
         <v>50</v>
       </c>
       <c r="E259">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -6840,7 +6840,7 @@
         <v>50</v>
       </c>
       <c r="E260">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>